<commit_message>
lots of things done!
</commit_message>
<xml_diff>
--- a/Documents/botPowerFactors.xlsx
+++ b/Documents/botPowerFactors.xlsx
@@ -339,25 +339,25 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>857</v>
+        <v>866</v>
       </c>
       <c r="B1">
-        <v>1663</v>
+        <v>1670</v>
       </c>
       <c r="C1">
         <f>B1-A1</f>
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E1">
         <f>C1/C2</f>
-        <v>4.03</v>
+        <v>5.36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -365,87 +365,87 @@
         <v>1000</v>
       </c>
       <c r="B2">
-        <v>1200</v>
+        <v>1150</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C14" si="0">B2-A2</f>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E2">
         <f>A1-A2*E1</f>
-        <v>-3173.0000000000005</v>
+        <v>-4494</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1737</v>
+        <v>1743</v>
       </c>
       <c r="B4">
-        <v>2323</v>
+        <v>2328</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E4">
         <f>C4/C5</f>
-        <v>1.9533333333333334</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1200</v>
+        <v>1150</v>
       </c>
       <c r="B5">
-        <v>1500</v>
+        <v>1400</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="E5">
         <f>A4-A5*E4</f>
-        <v>-607</v>
+        <v>-948</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2396</v>
+        <v>2401</v>
       </c>
       <c r="B7">
-        <v>2836</v>
+        <v>2839</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E7">
         <f>C7/C8</f>
-        <v>0.88</v>
+        <v>1.095</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1500</v>
+        <v>1400</v>
       </c>
       <c r="B8">
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E8">
         <f>A7-A8*E7</f>
-        <v>1076</v>
+        <v>868</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2910</v>
+        <v>2912</v>
       </c>
       <c r="B10">
-        <v>3349</v>
+        <v>3351</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -453,55 +453,55 @@
       </c>
       <c r="E10">
         <f>C10/C11</f>
-        <v>0.2195</v>
+        <v>0.878</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="B11">
-        <v>4000</v>
+        <v>2300</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="E11">
         <f>A10-A11*E10</f>
-        <v>2471</v>
+        <v>1331.6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3423</v>
+        <v>3424</v>
       </c>
       <c r="B13">
         <v>4009</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E13">
         <f>C13/C14</f>
-        <v>0.19533333333333333</v>
+        <v>0.12446808510638298</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4000</v>
+        <v>2300</v>
       </c>
       <c r="B14">
         <v>7000</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>4700</v>
       </c>
       <c r="E14">
         <f>A13-A14*E13</f>
-        <v>2641.6666666666665</v>
+        <v>3137.7234042553191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>